<commit_message>
backlog and springlog updated
</commit_message>
<xml_diff>
--- a/ch.bfh.btx8081.w2013.blue/doc/task09and10/task9&10_v2.0.2.xlsx
+++ b/ch.bfh.btx8081.w2013.blue/doc/task09and10/task9&10_v2.0.2.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1035" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="14220" windowHeight="3720"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" calcMode="manual" concurrentCalc="0"/>
+  <oleSize ref="A3:I4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -317,6 +318,12 @@
   </si>
   <si>
     <t>35h</t>
+  </si>
+  <si>
+    <t>When the patient denies drugs the doctor can enter when the patient does it and what drug. This will then be visible in the patientview.</t>
+  </si>
+  <si>
+    <t>If the patient must be referred, the doctor can click on the referral button and enter information about: during time, diagnosis, external clinic or doctor, name of the doctor, is it a FU or a normal referral,… after click on the button "send referral" the input will be writen to a txt. file. The referral is also visible in the patientview.</t>
   </si>
 </sst>
 </file>
@@ -747,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,14 +822,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
@@ -835,14 +844,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -900,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1373,7 @@
         <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
@@ -1572,7 +1583,7 @@
         <v>67</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
diary updated, sprint backlog, alertpanel angepasst
</commit_message>
<xml_diff>
--- a/ch.bfh.btx8081.w2013.blue/doc/task09and10/task9&10_v2.0.2.xlsx
+++ b/ch.bfh.btx8081.w2013.blue/doc/task09and10/task9&10_v2.0.2.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="360" windowWidth="25600" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="5430" windowHeight="5475"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="time schedule (quick and dirty)" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <oleSize ref="A1:P4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -89,9 +90,6 @@
     <t>80h</t>
   </si>
   <si>
-    <t>not started</t>
-  </si>
-  <si>
     <t>7 Wochen / Sprint</t>
   </si>
   <si>
@@ -317,7 +315,10 @@
     <t>not to be implemented</t>
   </si>
   <si>
-    <t>pending</t>
+    <t>45h</t>
+  </si>
+  <si>
+    <t>60h</t>
   </si>
 </sst>
 </file>
@@ -484,85 +485,63 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="55">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color theme="1"/>
@@ -928,23 +907,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="28">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -970,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="135" customHeight="1">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -978,7 +957,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -987,13 +966,16 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="112">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1001,7 +983,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -1010,14 +992,16 @@
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="42">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1025,7 +1009,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1033,13 +1017,17 @@
       <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -1064,27 +1052,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +1107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1127,16 +1115,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -1151,13 +1139,13 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -1165,16 +1153,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
         <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -1189,10 +1177,10 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -1200,16 +1188,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -1224,10 +1212,10 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -1235,16 +1223,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -1259,10 +1247,10 @@
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.5</v>
       </c>
@@ -1270,16 +1258,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -1294,10 +1282,10 @@
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.6</v>
       </c>
@@ -1305,16 +1293,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -1329,10 +1317,10 @@
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.7</v>
       </c>
@@ -1340,16 +1328,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -1364,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.8</v>
       </c>
@@ -1375,16 +1363,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1399,14 +1387,14 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="L9" s="9">
         <f>SUM(J2+J3+J4+J5+J6+J7)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="6" customHeight="1">
+    <row r="10" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1416,12 +1404,12 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:12" ht="28">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.1</v>
       </c>
@@ -1429,16 +1417,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
@@ -1453,10 +1441,10 @@
         <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.2000000000000002</v>
       </c>
@@ -1464,16 +1452,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
@@ -1488,10 +1476,10 @@
         <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.2999999999999998</v>
       </c>
@@ -1499,16 +1487,16 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
@@ -1523,10 +1511,10 @@
         <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2.4</v>
       </c>
@@ -1534,16 +1522,16 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -1558,10 +1546,10 @@
         <v>10</v>
       </c>
       <c r="K14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="42">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2.5</v>
       </c>
@@ -1569,16 +1557,16 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
@@ -1593,10 +1581,10 @@
         <v>4</v>
       </c>
       <c r="K15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.6</v>
       </c>
@@ -1604,16 +1592,16 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
         <v>91</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
-        <v>92</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
@@ -1628,10 +1616,10 @@
         <v>12</v>
       </c>
       <c r="K16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2.7</v>
       </c>
@@ -1639,16 +1627,16 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
         <v>6</v>
@@ -1663,10 +1651,10 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2.8</v>
       </c>
@@ -1674,16 +1662,16 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
@@ -1698,10 +1686,10 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.9</v>
       </c>
@@ -1709,16 +1697,16 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -1733,14 +1721,14 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="L19" s="9">
         <f>SUM(J11+J12+J13+J14+J15+J16+J17)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="6" customHeight="1">
+    <row r="20" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1753,7 +1741,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:12" ht="28">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3.1</v>
       </c>
@@ -1761,16 +1749,16 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>
@@ -1782,10 +1770,10 @@
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3.2</v>
       </c>
@@ -1793,16 +1781,16 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
@@ -1814,10 +1802,10 @@
         <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="28">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3.3</v>
       </c>
@@ -1825,16 +1813,16 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
@@ -1846,10 +1834,10 @@
         <v>6</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="28">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3.4</v>
       </c>
@@ -1857,16 +1845,16 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
@@ -1878,10 +1866,10 @@
         <v>8</v>
       </c>
       <c r="K24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="28">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3.5</v>
       </c>
@@ -1889,16 +1877,16 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G25" t="s">
         <v>6</v>
@@ -1910,10 +1898,10 @@
         <v>2</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3.6</v>
       </c>
@@ -1921,16 +1909,16 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
         <v>6</v>
@@ -1942,10 +1930,10 @@
         <v>5</v>
       </c>
       <c r="K26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3.7</v>
       </c>
@@ -1953,16 +1941,16 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" t="s">
         <v>6</v>
@@ -1974,31 +1962,31 @@
         <v>7</v>
       </c>
       <c r="K27" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K15:K19 K2:K12 K21:K27">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="not started">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="not started">
       <formula>NOT(ISERROR(SEARCH("not started",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="finished">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="finished">
       <formula>NOT(ISERROR(SEARCH("finished",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K14">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="not started">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="not started">
       <formula>NOT(ISERROR(SEARCH("not started",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="finished">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="finished">
       <formula>NOT(ISERROR(SEARCH("finished",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="not started">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="not started">
       <formula>NOT(ISERROR(SEARCH("not started",K20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="finished">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="finished">
       <formula>NOT(ISERROR(SEARCH("finished",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2020,90 +2008,90 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:15">
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="3:15">
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
       </c>
       <c r="K3">
         <v>8.75</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="3:15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="K4">
         <v>70</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="3:15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5">
         <v>6</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="K6">
         <v>1.75</v>
       </c>
       <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" t="s">
         <v>31</v>
       </c>
-      <c r="O6" t="s">
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="3:15">
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="3:15">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15">
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="3:15">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>280</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18">
         <v>40</v>

</xml_diff>